<commit_message>
added mysheet["mynamedrange"] support for Excel on the web
</commit_message>
<xml_diff>
--- a/tests/test_json/json.xlsx
+++ b/tests/test_json/json.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/test_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B754D06-3B75-604D-BA26-D9898E1F3E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32902394-7514-6545-A425-3CBF8F9E41E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{122BE06B-C62B-364D-8C27-94A5A3A52BCE}"/>
   </bookViews>
@@ -17,7 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="one">Sheet1!$A$1</definedName>
+    <definedName name="two" localSheetId="0">Sheet1!$C$7:$D$8</definedName>
+    <definedName name="two">Sheet2!$A$1:$A$2</definedName>
+  </definedNames>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,9 +100,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -432,7 +436,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -444,7 +448,7 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>44197</v>
       </c>
     </row>
@@ -452,19 +456,19 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -477,7 +481,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,10 +544,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>44470</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>44561.982638888891</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remote Interpreter: Add support for mysheet["my_named_range"] syntax (#1975)
* added mysheet["mynamedrange"] support for remote interpreter (backend and desktop Excel)

* added mysheet["mynamedrange"] support for Google Sheets

* added mysheet["mynamedrange"] support for Excel on the web

* remote engine: error handling for non existent string addresses
</commit_message>
<xml_diff>
--- a/tests/test_json/json.xlsx
+++ b/tests/test_json/json.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/test_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B754D06-3B75-604D-BA26-D9898E1F3E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32902394-7514-6545-A425-3CBF8F9E41E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{122BE06B-C62B-364D-8C27-94A5A3A52BCE}"/>
   </bookViews>
@@ -17,7 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="one">Sheet1!$A$1</definedName>
+    <definedName name="two" localSheetId="0">Sheet1!$C$7:$D$8</definedName>
+    <definedName name="two">Sheet2!$A$1:$A$2</definedName>
+  </definedNames>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,9 +100,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -432,7 +436,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -444,7 +448,7 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>44197</v>
       </c>
     </row>
@@ -452,19 +456,19 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -477,7 +481,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,10 +544,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>44470</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>44561.982638888891</v>
       </c>
     </row>

</xml_diff>